<commit_message>
this is sencond commit
</commit_message>
<xml_diff>
--- a/MyExcel.xlsx
+++ b/MyExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>as</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>sa</t>
+  </si>
+  <si>
+    <t>ikljkljkljkl</t>
   </si>
 </sst>
 </file>
@@ -359,20 +362,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -380,12 +383,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:5">
       <c r="D6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="7" spans="2:5">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>2</v>
       </c>

</xml_diff>